<commit_message>
update DFR and PQ Config templates and examples
</commit_message>
<xml_diff>
--- a/Source/Documentation/Device Definitions Examples & Templates/openXDA Configuration Template - PQ.xlsx
+++ b/Source/Documentation/Device Definitions Examples & Templates/openXDA Configuration Template - PQ.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Products\openXDA\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gpa.gridprotectionalliance.org\GPA\Share\Products\openXDA\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="9540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15615" windowHeight="11580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analytics (optional)" sheetId="1" r:id="rId1"/>
@@ -133,12 +133,6 @@
   </si>
   <si>
     <t>stationLongitude</t>
-  </si>
-  <si>
-    <t>Specific information about the reporting device; PQ Monitor etc. Up to 200 alphanumeric characters for each field.</t>
-  </si>
-  <si>
-    <t>This template is intended for use in configuring an openXDA database for PQ devices. Each device must be defined by specifying the information described below. Please enter a value for each parameter. "ID" fields are limited to 50 alphanumeric characters, other non-numeric fields can contain up to 200 alphanumeric characters.</t>
   </si>
   <si>
     <t>Unique ID for the location of the device: Up to 50 alphanumeric characters.</t>
@@ -224,6 +218,12 @@
   </si>
   <si>
     <t>Zero sequence reactance: nummeric decimal value</t>
+  </si>
+  <si>
+    <t>This template is intended for use in configuring an openXDA database for data from substation devices such as PQ monitors or relays; one device per template. A separate template is available for DFRs. Each device must be defined by specifying the information described below. Please enter a value for each parameter. "ID" fields are limited to 50 alphanumeric characters, other non-numeric fields can contain up to 200 alphanumeric characters.</t>
+  </si>
+  <si>
+    <t>Specific information about the reporting device; PQ Monitor etc. Up to 200 alphanumeric characters each for make and model fields.</t>
   </si>
 </sst>
 </file>
@@ -1033,12 +1033,44 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1049,6 +1081,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1084,6 +1134,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1111,82 +1173,20 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1514,57 +1514,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1631,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,171 +1645,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="A1" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="65"/>
       <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="68"/>
       <c r="L2" s="35"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="68"/>
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="35"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C6" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="36"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="36"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="54" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="20"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="90"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="47"/>
       <c r="M7" s="20"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L8" s="36"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="47"/>
       <c r="M8" s="20"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
       <c r="L9" s="36"/>
       <c r="M9" s="20"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="20"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="71" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="20"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="75" t="s">
-        <v>38</v>
-      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="76"/>
       <c r="E12" s="76"/>
       <c r="F12" s="76"/>
@@ -1818,343 +1813,362 @@
       <c r="I12" s="76"/>
       <c r="J12" s="76"/>
       <c r="K12" s="77"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="78" t="s">
+      <c r="L12" s="48"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="87" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="89"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="57" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="91"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="91"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="59"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="36"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="36"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="79"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="57" t="s">
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="37"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="79"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="82" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="84"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L16" s="36"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="36"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="56" t="s">
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="38"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="37"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="41" t="s">
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="38"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="38"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="38"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="28"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="29"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="28"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="29"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="29"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="22"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="54"/>
       <c r="L24" s="29"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="87" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="89"/>
-      <c r="L25" s="29"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="29"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="85"/>
-      <c r="J26" s="85"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="29"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>23</v>
-      </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="42"/>
+      <c r="C27" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="52"/>
       <c r="L27" s="29"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="29"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="29"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="29"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="29"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="B30" s="27"/>
+      <c r="C30" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="29"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="30"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="33"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="30"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C15:K15"/>
-    <mergeCell ref="C25:K25"/>
-    <mergeCell ref="A1:K3"/>
-    <mergeCell ref="C6:K7"/>
-    <mergeCell ref="C10:K11"/>
-    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="A1:K4"/>
+    <mergeCell ref="C7:K8"/>
+    <mergeCell ref="C11:K12"/>
     <mergeCell ref="C19:K19"/>
     <mergeCell ref="C20:K20"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C27:K27"/>
+    <mergeCell ref="C28:K28"/>
+    <mergeCell ref="C29:K29"/>
+    <mergeCell ref="C30:K30"/>
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="C26:K26"/>
     <mergeCell ref="C21:K21"/>
     <mergeCell ref="C22:K22"/>
     <mergeCell ref="C23:K23"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="C17:K17"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="C14:K14"/>
-    <mergeCell ref="C26:K26"/>
-    <mergeCell ref="C27:K27"/>
-    <mergeCell ref="C28:K28"/>
-    <mergeCell ref="C29:K29"/>
+    <mergeCell ref="C24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>